<commit_message>
updated data analysis for granger causality
</commit_message>
<xml_diff>
--- a/analysis/ResultsAnalysis.xlsx
+++ b/analysis/ResultsAnalysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irenedelatorre/webhoseAPI/projectWork/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irenedelatorre/webhoseAPI/projectWork/github_folder/Social-Media-Impact-on-Stock-Market-and-Price/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="460" windowWidth="23660" windowHeight="16500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="18980" windowHeight="16500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="42">
   <si>
     <t>Data Correlation Result</t>
   </si>
@@ -158,6 +158,9 @@
   <si>
     <t>AVERAGE</t>
   </si>
+  <si>
+    <t>Timewarner</t>
+  </si>
 </sst>
 </file>
 
@@ -256,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -307,6 +310,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +373,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1002,11 +1008,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-1994158720"/>
-        <c:axId val="-1994161856"/>
+        <c:axId val="2130944256"/>
+        <c:axId val="2130947504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1994158720"/>
+        <c:axId val="2130944256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994161856"/>
+        <c:crossAx val="2130947504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1057,7 +1063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1994161856"/>
+        <c:axId val="2130947504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994158720"/>
+        <c:crossAx val="2130944256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1201,7 +1207,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1837,11 +1842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-1994206464"/>
-        <c:axId val="-1994208368"/>
+        <c:axId val="2131053248"/>
+        <c:axId val="2131056480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1994206464"/>
+        <c:axId val="2131053248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,7 +1888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994208368"/>
+        <c:crossAx val="2131056480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1891,7 +1896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1994208368"/>
+        <c:axId val="2131056480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994206464"/>
+        <c:crossAx val="2131053248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2035,7 +2040,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2682,11 +2686,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="4"/>
-        <c:axId val="-1994372656"/>
-        <c:axId val="-1994376064"/>
+        <c:axId val="2111371120"/>
+        <c:axId val="2111374352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1994372656"/>
+        <c:axId val="2111371120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,7 +2732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994376064"/>
+        <c:crossAx val="2111374352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2736,7 +2740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1994376064"/>
+        <c:axId val="2111374352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2786,7 +2790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994372656"/>
+        <c:crossAx val="2111371120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2875,7 +2879,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3521,11 +3524,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2079508048"/>
-        <c:axId val="-2079541712"/>
+        <c:axId val="2131098560"/>
+        <c:axId val="2131101792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079508048"/>
+        <c:axId val="2131098560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3568,7 +3571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079541712"/>
+        <c:crossAx val="2131101792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3576,7 +3579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079541712"/>
+        <c:axId val="2131101792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3627,7 +3630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079508048"/>
+        <c:crossAx val="2131098560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7468,10 +7471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7923,31 +7926,169 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="20">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="D21" s="16">
+        <v>8</v>
+      </c>
+      <c r="E21" s="19">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="F21" s="16">
+        <v>7</v>
+      </c>
+      <c r="G21" s="19">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="H21" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="19">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D22" s="16">
+        <v>4</v>
+      </c>
+      <c r="E22" s="19">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="F22" s="16">
+        <v>4</v>
+      </c>
+      <c r="G22" s="19">
+        <v>1.17E-2</v>
+      </c>
+      <c r="H22" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="16">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="D23" s="16">
+        <v>8</v>
+      </c>
+      <c r="E23" s="19">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F23" s="16">
+        <v>7</v>
+      </c>
+      <c r="G23" s="19">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H23" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="19">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="D24" s="16">
+        <v>8</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="F24" s="16">
+        <v>8</v>
+      </c>
+      <c r="G24" s="19">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="H24" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D25" s="16">
+        <v>8</v>
+      </c>
+      <c r="E25" s="16">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="F25" s="16">
+        <v>5</v>
+      </c>
+      <c r="G25" s="19">
+        <v>1.06E-2</v>
+      </c>
+      <c r="H25" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D26" s="16">
+        <v>7</v>
+      </c>
+      <c r="E26" s="19">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <v>8</v>
+      </c>
+      <c r="G26" s="16">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H26" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="14">
-        <f>AVERAGE(C3:C20)</f>
-        <v>7.3494444444444459E-2</v>
-      </c>
-      <c r="D21" s="14">
-        <f>AVERAGE(D3:D20)</f>
-        <v>5.5</v>
-      </c>
-      <c r="E21" s="14">
-        <f>AVERAGE(E3:E20)</f>
-        <v>9.4133333333333333E-2</v>
-      </c>
-      <c r="F21" s="14">
-        <f>AVERAGE(F3:F20)</f>
-        <v>5.7777777777777777</v>
-      </c>
-      <c r="G21" s="14">
-        <f>AVERAGE(G3:G20)</f>
-        <v>7.3033333333333339E-2</v>
-      </c>
-      <c r="H21" s="14">
-        <f>AVERAGE(H3:H20)</f>
+      <c r="C27" s="14">
+        <f>AVERAGE(C3:C26)</f>
+        <v>6.266666666666669E-2</v>
+      </c>
+      <c r="D27" s="14">
+        <f>AVERAGE(D3:D26)</f>
+        <v>5.916666666666667</v>
+      </c>
+      <c r="E27" s="14">
+        <f t="shared" ref="E27:H27" si="0">AVERAGE(E3:E26)</f>
+        <v>9.8420833333333332E-2</v>
+      </c>
+      <c r="F27" s="14">
+        <f t="shared" si="0"/>
+        <v>5.958333333333333</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" si="0"/>
+        <v>6.3112500000000002E-2</v>
+      </c>
+      <c r="H27" s="14">
+        <f t="shared" si="0"/>
         <v>5.666666666666667</v>
       </c>
     </row>

</xml_diff>